<commit_message>
BACE-29: Add option to toggle display of posterior estimates to field plug-in
</commit_message>
<xml_diff>
--- a/integration/SurveyCTO/BACE_template.xlsx
+++ b/integration/SurveyCTO/BACE_template.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26224" uniqueCount="460">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30881" uniqueCount="466">
   <si>
     <t>type</t>
   </si>
@@ -2959,6 +2959,24 @@
   </si>
   <si>
     <t>2401271951</t>
+  </si>
+  <si>
+    <t>2401271952</t>
+  </si>
+  <si>
+    <t>2401271953</t>
+  </si>
+  <si>
+    <t>display_estimates_page</t>
+  </si>
+  <si>
+    <t>custom-bace(bace_url=${bace_url}, unique_profile_id=${unique_profile_id}, final_question = ${final_question}, previous_choice = ${previous_choice}, display_estimates_page = ${display_estimates_page})</t>
+  </si>
+  <si>
+    <t>2401271954</t>
+  </si>
+  <si>
+    <t>2401271955</t>
   </si>
 </sst>
 </file>
@@ -5381,13 +5399,13 @@
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="6" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>49</v>
+        <v>462</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="D15" s="8" t="s">
         <v>25</v>
@@ -5420,7 +5438,7 @@
         <v>25</v>
       </c>
       <c r="N15" s="6" t="s">
-        <v>25</v>
+        <v>106</v>
       </c>
       <c r="O15" s="6" t="s">
         <v>25</v>
@@ -5458,10 +5476,10 @@
         <v>48</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D16" s="8" t="s">
         <v>25</v>
@@ -5529,13 +5547,13 @@
     </row>
     <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="10" t="s">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>451</v>
+        <v>52</v>
       </c>
       <c r="D17" s="8" t="s">
         <v>25</v>
@@ -5559,7 +5577,7 @@
         <v>25</v>
       </c>
       <c r="K17" s="10" t="s">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="L17" s="6" t="s">
         <v>25</v>
@@ -5603,13 +5621,13 @@
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="10" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D18" s="8" t="s">
         <v>25</v>
@@ -5633,7 +5651,7 @@
         <v>25</v>
       </c>
       <c r="K18" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="L18" s="6" t="s">
         <v>25</v>
@@ -5677,13 +5695,13 @@
     </row>
     <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="10" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>25</v>
+        <v>452</v>
       </c>
       <c r="D19" s="8" t="s">
         <v>25</v>
@@ -5707,7 +5725,7 @@
         <v>25</v>
       </c>
       <c r="K19" s="6" t="s">
-        <v>25</v>
+        <v>59</v>
       </c>
       <c r="L19" s="6" t="s">
         <v>25</v>
@@ -5751,13 +5769,13 @@
     </row>
     <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>63</v>
+        <v>25</v>
       </c>
       <c r="D20" s="8" t="s">
         <v>25</v>
@@ -5793,7 +5811,7 @@
         <v>25</v>
       </c>
       <c r="O20" s="11" t="s">
-        <v>64</v>
+        <v>25</v>
       </c>
       <c r="P20" s="6" t="s">
         <v>25</v>
@@ -5825,13 +5843,13 @@
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="10" t="s">
-        <v>32</v>
+        <v>61</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>25</v>
+        <v>63</v>
       </c>
       <c r="D21" s="8" t="s">
         <v>25</v>
@@ -5864,10 +5882,10 @@
         <v>25</v>
       </c>
       <c r="N21" s="6" t="s">
-        <v>443</v>
+        <v>25</v>
       </c>
       <c r="O21" s="6" t="s">
-        <v>25</v>
+        <v>64</v>
       </c>
       <c r="P21" s="6" t="s">
         <v>25</v>
@@ -5902,7 +5920,7 @@
         <v>32</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C22" s="10" t="s">
         <v>25</v>
@@ -5938,7 +5956,7 @@
         <v>25</v>
       </c>
       <c r="N22" s="11" t="s">
-        <v>70</v>
+        <v>443</v>
       </c>
       <c r="O22" s="6" t="s">
         <v>25</v>
@@ -5976,7 +5994,7 @@
         <v>32</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C23" s="7" t="s">
         <v>25</v>
@@ -6012,7 +6030,7 @@
         <v>25</v>
       </c>
       <c r="N23" s="6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="O23" s="6" t="s">
         <v>25</v>
@@ -6047,13 +6065,13 @@
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="12" t="s">
-        <v>73</v>
+        <v>32</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>453</v>
+        <v>25</v>
       </c>
       <c r="D24" s="15" t="s">
         <v>25</v>
@@ -6062,7 +6080,7 @@
         <v>25</v>
       </c>
       <c r="F24" s="15" t="s">
-        <v>445</v>
+        <v>25</v>
       </c>
       <c r="G24" s="15" t="s">
         <v>25</v>
@@ -6077,7 +6095,7 @@
         <v>25</v>
       </c>
       <c r="K24" s="15" t="s">
-        <v>59</v>
+        <v>25</v>
       </c>
       <c r="L24" s="15" t="s">
         <v>25</v>
@@ -6086,7 +6104,7 @@
         <v>25</v>
       </c>
       <c r="N24" s="16" t="s">
-        <v>25</v>
+        <v>72</v>
       </c>
       <c r="O24" s="15" t="s">
         <v>25</v>
@@ -6121,13 +6139,13 @@
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="10" t="s">
-        <v>19</v>
+        <v>73</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D25" s="8" t="s">
         <v>25</v>
@@ -6136,7 +6154,7 @@
         <v>25</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>25</v>
+        <v>463</v>
       </c>
       <c r="G25" s="6" t="s">
         <v>25</v>
@@ -6151,7 +6169,7 @@
         <v>25</v>
       </c>
       <c r="K25" s="6" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="L25" s="6" t="s">
         <v>25</v>
@@ -6195,13 +6213,13 @@
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="10" t="s">
-        <v>48</v>
+        <v>19</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>79</v>
+        <v>454</v>
       </c>
       <c r="D26" s="8" t="s">
         <v>25</v>
@@ -6225,7 +6243,7 @@
         <v>25</v>
       </c>
       <c r="K26" s="6" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="L26" s="6" t="s">
         <v>25</v>
@@ -6269,13 +6287,13 @@
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="10" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>25</v>
+        <v>79</v>
       </c>
       <c r="D27" s="8" t="s">
         <v>25</v>
@@ -6308,7 +6326,7 @@
         <v>25</v>
       </c>
       <c r="N27" s="10" t="s">
-        <v>427</v>
+        <v>25</v>
       </c>
       <c r="O27" s="6" t="s">
         <v>25</v>
@@ -6346,7 +6364,7 @@
         <v>32</v>
       </c>
       <c r="B28" s="18" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C28" s="14" t="s">
         <v>25</v>
@@ -6382,7 +6400,7 @@
         <v>25</v>
       </c>
       <c r="N28" s="19" t="s">
-        <v>85</v>
+        <v>427</v>
       </c>
       <c r="O28" s="20" t="s">
         <v>25</v>
@@ -6420,7 +6438,7 @@
         <v>32</v>
       </c>
       <c r="B29" s="18" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C29" s="14" t="s">
         <v>25</v>
@@ -6456,7 +6474,7 @@
         <v>25</v>
       </c>
       <c r="N29" s="19" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="O29" s="20" t="s">
         <v>25</v>
@@ -6494,7 +6512,7 @@
         <v>32</v>
       </c>
       <c r="B30" s="18" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C30" s="14" t="s">
         <v>25</v>
@@ -6530,7 +6548,7 @@
         <v>25</v>
       </c>
       <c r="N30" s="19" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="O30" s="20" t="s">
         <v>25</v>
@@ -6568,7 +6586,7 @@
         <v>32</v>
       </c>
       <c r="B31" s="18" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C31" s="14" t="s">
         <v>25</v>
@@ -6604,7 +6622,7 @@
         <v>25</v>
       </c>
       <c r="N31" s="19" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="O31" s="20" t="s">
         <v>25</v>
@@ -6642,7 +6660,7 @@
         <v>32</v>
       </c>
       <c r="B32" s="18" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C32" s="14" t="s">
         <v>25</v>
@@ -6678,7 +6696,7 @@
         <v>25</v>
       </c>
       <c r="N32" s="19" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="O32" s="20" t="s">
         <v>25</v>
@@ -6716,7 +6734,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="18" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C33" s="14" t="s">
         <v>25</v>
@@ -6752,7 +6770,7 @@
         <v>25</v>
       </c>
       <c r="N33" s="19" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="O33" s="20" t="s">
         <v>25</v>
@@ -6790,7 +6808,7 @@
         <v>32</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>432</v>
+        <v>94</v>
       </c>
       <c r="C34" s="10" t="s">
         <v>25</v>
@@ -6826,7 +6844,7 @@
         <v>25</v>
       </c>
       <c r="N34" s="11" t="s">
-        <v>433</v>
+        <v>95</v>
       </c>
       <c r="O34" s="6" t="s">
         <v>25</v>
@@ -6864,7 +6882,7 @@
         <v>32</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="C35" s="7" t="s">
         <v>25</v>
@@ -6900,7 +6918,7 @@
         <v>25</v>
       </c>
       <c r="N35" s="11" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="O35" s="6" t="s">
         <v>25</v>
@@ -6938,7 +6956,7 @@
         <v>32</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="C36" s="7" t="s">
         <v>25</v>
@@ -6974,7 +6992,7 @@
         <v>25</v>
       </c>
       <c r="N36" s="6" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="O36" s="6" t="s">
         <v>25</v>
@@ -7012,7 +7030,7 @@
         <v>32</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>96</v>
+        <v>436</v>
       </c>
       <c r="C37" s="7" t="s">
         <v>25</v>
@@ -7048,7 +7066,7 @@
         <v>25</v>
       </c>
       <c r="N37" s="6" t="s">
-        <v>97</v>
+        <v>437</v>
       </c>
       <c r="O37" s="6" t="s">
         <v>25</v>
@@ -7083,13 +7101,13 @@
     </row>
     <row r="38" ht="15.75" customHeight="1">
       <c r="A38" s="6" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>455</v>
+        <v>25</v>
       </c>
       <c r="D38" s="8" t="s">
         <v>25</v>
@@ -7113,7 +7131,7 @@
         <v>25</v>
       </c>
       <c r="K38" s="6" t="s">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="L38" s="6" t="s">
         <v>25</v>
@@ -7122,7 +7140,7 @@
         <v>25</v>
       </c>
       <c r="N38" s="6" t="s">
-        <v>25</v>
+        <v>97</v>
       </c>
       <c r="O38" s="6" t="s">
         <v>25</v>
@@ -7157,13 +7175,13 @@
     </row>
     <row r="39" ht="15.75" customHeight="1">
       <c r="A39" s="6" t="s">
-        <v>60</v>
+        <v>19</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>78</v>
+        <v>98</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>25</v>
+        <v>455</v>
       </c>
       <c r="D39" s="8" t="s">
         <v>25</v>
@@ -7187,7 +7205,7 @@
         <v>25</v>
       </c>
       <c r="K39" s="6" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="L39" s="6" t="s">
         <v>25</v>
@@ -7231,10 +7249,10 @@
     </row>
     <row r="40" ht="15.75" customHeight="1">
       <c r="A40" s="6" t="s">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>62</v>
+        <v>78</v>
       </c>
       <c r="C40" s="7" t="s">
         <v>25</v>
@@ -7305,10 +7323,10 @@
     </row>
     <row r="41" ht="15.75" customHeight="1">
       <c r="A41" s="6" t="s">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="C41" s="7" t="s">
         <v>25</v>
@@ -7378,29 +7396,75 @@
       <c r="Z41" s="9"/>
     </row>
     <row r="42" ht="15.75" customHeight="1">
-      <c r="A42" s="6"/>
-      <c r="B42" s="6"/>
-      <c r="C42" s="7"/>
-      <c r="D42" s="8"/>
-      <c r="E42" s="6"/>
-      <c r="F42" s="6"/>
-      <c r="G42" s="6"/>
-      <c r="H42" s="8"/>
-      <c r="I42" s="6"/>
-      <c r="J42" s="6"/>
-      <c r="K42" s="6"/>
-      <c r="L42" s="6"/>
-      <c r="M42" s="6"/>
-      <c r="N42" s="6"/>
-      <c r="O42" s="6"/>
-      <c r="P42" s="6"/>
-      <c r="Q42" s="6"/>
-      <c r="R42" s="6"/>
-      <c r="S42" s="6"/>
-      <c r="T42" s="6"/>
-      <c r="U42" s="6"/>
-      <c r="V42" s="6"/>
-      <c r="W42" s="6"/>
+      <c r="A42" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D42" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E42" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F42" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G42" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H42" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I42" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="J42" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="K42" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="L42" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="M42" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="N42" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="O42" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="P42" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q42" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="R42" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="S42" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="T42" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="U42" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="V42" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="W42" s="6" t="s">
+        <v>25</v>
+      </c>
       <c r="X42" s="9"/>
       <c r="Y42" s="9"/>
       <c r="Z42" s="9"/>
@@ -20975,7 +21039,7 @@
         <v>117</v>
       </c>
       <c r="C2" s="26" t="s">
-        <v>459</v>
+        <v>465</v>
       </c>
       <c r="D2" s="27" t="s">
         <v>25</v>

</xml_diff>